<commit_message>
added devices to BU and buildings
</commit_message>
<xml_diff>
--- a/Approximationen/AC Kosten.xlsx
+++ b/Approximationen/AC Kosten.xlsx
@@ -5,13 +5,13 @@
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="7" documentId="11_EB6B1133B04C936C96366B20EDBDEFCCDC1637D8" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{3CA93CB4-C292-4BFC-A26C-E7B3505EA5E6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagramm" sheetId="2" r:id="rId1"/>
     <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>